<commit_message>
- code update for lease, royaltymaster and well.
</commit_message>
<xml_diff>
--- a/excel-app/database.xlsx
+++ b/excel-app/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="183">
   <si>
     <t>Lease Type</t>
   </si>
@@ -565,6 +565,18 @@
   </si>
   <si>
     <t xml:space="preserve">(Sask Oil SKProvCrownVar / SaskWellHead / No Deductions / Fourth Tier </t>
+  </si>
+  <si>
+    <t>(Used for testing well update</t>
+  </si>
+  <si>
+    <t>OL-3000</t>
+  </si>
+  <si>
+    <t>(Used to test Royalty Maser Tests</t>
+  </si>
+  <si>
+    <t>(Used to test update</t>
   </si>
 </sst>
 </file>
@@ -6009,10 +6021,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6026,7 +6038,7 @@
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -6054,8 +6066,11 @@
       <c r="I1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6084,7 +6099,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6110,7 +6125,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6133,7 +6148,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6159,7 +6174,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6179,7 +6194,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6199,7 +6214,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6217,6 +6232,29 @@
       </c>
       <c r="G8" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9">
+        <v>1.2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>163</v>
+      </c>
+      <c r="J9" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -6226,10 +6264,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6240,7 +6278,7 @@
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>144</v>
       </c>
@@ -6253,8 +6291,11 @@
       <c r="D1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>139</v>
       </c>
@@ -6268,7 +6309,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>140</v>
       </c>
@@ -6282,7 +6323,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>141</v>
       </c>
@@ -6296,7 +6337,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>142</v>
       </c>
@@ -6310,7 +6351,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>143</v>
       </c>
@@ -6324,7 +6365,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>171</v>
       </c>
@@ -6338,7 +6379,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>175</v>
       </c>
@@ -6350,6 +6391,23 @@
       </c>
       <c r="D8">
         <v>2345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9">
+        <v>123</v>
+      </c>
+      <c r="D9">
+        <v>2345</v>
+      </c>
+      <c r="E9" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -6359,11 +6417,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7264,6 +7322,32 @@
       </c>
       <c r="I30" s="17">
         <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3000</v>
+      </c>
+      <c r="B31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="I31" s="17">
+        <v>1</v>
+      </c>
+      <c r="J31" s="18">
+        <v>40513</v>
+      </c>
+      <c r="L31" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -9021,7 +9105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Update attribute name
</commit_message>
<xml_diff>
--- a/excel-app/database.xlsx
+++ b/excel-app/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="172">
   <si>
     <t>Lease Type</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Prov</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>ProdVol</t>
   </si>
   <si>
-    <t>SalesVol</t>
-  </si>
-  <si>
     <t>AecoCIndexPrice</t>
   </si>
   <si>
@@ -432,9 +426,6 @@
     <t>UWI</t>
   </si>
   <si>
-    <t>SalesPrice</t>
-  </si>
-  <si>
     <t>TransPrice</t>
   </si>
   <si>
@@ -447,24 +438,6 @@
     <t>CrownMultiplier</t>
   </si>
   <si>
-    <t>OL-0001</t>
-  </si>
-  <si>
-    <t>OL-0002</t>
-  </si>
-  <si>
-    <t>OL-0003</t>
-  </si>
-  <si>
-    <t>OL-0004</t>
-  </si>
-  <si>
-    <t>OL-0005</t>
-  </si>
-  <si>
-    <t>Lease</t>
-  </si>
-  <si>
     <t>SKWI111062705025W300</t>
   </si>
   <si>
@@ -543,9 +516,6 @@
     <t>SKProvCrownVar</t>
   </si>
   <si>
-    <t>OL-0006</t>
-  </si>
-  <si>
     <t>Regulation1995</t>
   </si>
   <si>
@@ -555,9 +525,6 @@
     <t>ReferencePrice</t>
   </si>
   <si>
-    <t>OL-2000</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -570,13 +537,13 @@
     <t>(Used for testing well update</t>
   </si>
   <si>
-    <t>OL-3000</t>
-  </si>
-  <si>
     <t>(Used to test Royalty Maser Tests</t>
   </si>
   <si>
     <t>(Used to test update</t>
+  </si>
+  <si>
+    <t>LeaseID</t>
   </si>
 </sst>
 </file>
@@ -620,7 +587,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -705,11 +672,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -755,6 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1402,102 +1379,102 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" t="s">
-        <v>88</v>
-      </c>
       <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>107</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>108</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>109</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>110</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>115</v>
+      </c>
+      <c r="R1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" t="s">
+        <v>118</v>
+      </c>
+      <c r="U1" t="s">
+        <v>127</v>
+      </c>
+      <c r="V1" t="s">
         <v>111</v>
       </c>
-      <c r="P1" t="s">
+      <c r="W1" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" t="s">
-        <v>117</v>
-      </c>
-      <c r="R1" t="s">
-        <v>118</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>119</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>120</v>
       </c>
-      <c r="U1" t="s">
-        <v>129</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE1" t="s">
         <v>113</v>
-      </c>
-      <c r="W1" t="s">
-        <v>114</v>
-      </c>
-      <c r="X1" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>124</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2">
         <v>201509</v>
@@ -1592,7 +1569,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3">
         <v>201508</v>
@@ -1687,7 +1664,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4">
         <v>201507</v>
@@ -1782,7 +1759,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5">
         <v>201506</v>
@@ -1877,7 +1854,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>201505</v>
@@ -1972,7 +1949,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B7">
         <v>201504</v>
@@ -2067,7 +2044,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8">
         <v>201503</v>
@@ -2162,7 +2139,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9">
         <v>201502</v>
@@ -2257,7 +2234,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B10">
         <v>201501</v>
@@ -2352,7 +2329,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B11">
         <v>201412</v>
@@ -2447,7 +2424,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B12">
         <v>201411</v>
@@ -2542,7 +2519,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13">
         <v>201410</v>
@@ -2637,7 +2614,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14">
         <v>201409</v>
@@ -2732,7 +2709,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B15">
         <v>201408</v>
@@ -2827,7 +2804,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16">
         <v>201407</v>
@@ -2922,7 +2899,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B17">
         <v>201406</v>
@@ -3017,7 +2994,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B18">
         <v>201405</v>
@@ -3112,7 +3089,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B19">
         <v>201404</v>
@@ -3207,7 +3184,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B20">
         <v>201403</v>
@@ -3302,7 +3279,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B21">
         <v>201402</v>
@@ -3397,7 +3374,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B22">
         <v>201401</v>
@@ -3492,7 +3469,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23">
         <v>201312</v>
@@ -3587,7 +3564,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24">
         <v>201311</v>
@@ -3682,7 +3659,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B25">
         <v>201310</v>
@@ -3777,7 +3754,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B26">
         <v>201309</v>
@@ -3872,7 +3849,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B27">
         <v>201308</v>
@@ -3967,7 +3944,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B28">
         <v>201307</v>
@@ -4062,7 +4039,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B29">
         <v>201306</v>
@@ -4157,7 +4134,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B30">
         <v>201305</v>
@@ -4252,7 +4229,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B31">
         <v>201304</v>
@@ -4347,7 +4324,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B32">
         <v>201303</v>
@@ -4442,7 +4419,7 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B33">
         <v>201302</v>
@@ -4537,7 +4514,7 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B34">
         <v>201301</v>
@@ -4632,7 +4609,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35">
         <v>201212</v>
@@ -4727,7 +4704,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B36">
         <v>201211</v>
@@ -4822,7 +4799,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B37">
         <v>201210</v>
@@ -4917,7 +4894,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B38">
         <v>201209</v>
@@ -5012,7 +4989,7 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B39">
         <v>201208</v>
@@ -5107,7 +5084,7 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40">
         <v>201207</v>
@@ -5202,7 +5179,7 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B41">
         <v>201206</v>
@@ -5297,7 +5274,7 @@
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B42">
         <v>201205</v>
@@ -5392,7 +5369,7 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B43">
         <v>201204</v>
@@ -5487,7 +5464,7 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B44">
         <v>201203</v>
@@ -5582,7 +5559,7 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B45">
         <v>201202</v>
@@ -5677,7 +5654,7 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B46">
         <v>201201</v>
@@ -5772,7 +5749,7 @@
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B47">
         <v>201112</v>
@@ -5867,7 +5844,7 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B48">
         <v>201111</v>
@@ -5983,35 +5960,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6024,12 +6001,12 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
@@ -6039,49 +6016,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" t="s">
         <v>144</v>
       </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" t="s">
-        <v>153</v>
-      </c>
       <c r="G1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="H1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="16">
         <v>1</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E2">
         <v>1.2</v>
@@ -6090,27 +6067,27 @@
         <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="H2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>140</v>
+      <c r="B3" s="16">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E3">
         <v>1.1000000000000001</v>
@@ -6119,142 +6096,142 @@
         <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16">
         <v>3</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E4">
         <v>0.9</v>
       </c>
       <c r="G4" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="I4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="16">
         <v>4</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>142</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E5">
         <v>1.25</v>
       </c>
       <c r="G5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="16">
         <v>5</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>143</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E6">
         <v>0.85</v>
       </c>
       <c r="G6" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16">
         <v>6</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>171</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>175</v>
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2000</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E8">
         <v>1.2</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>180</v>
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16">
+        <v>3000</v>
       </c>
       <c r="C9" t="s">
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E9">
         <v>1.2</v>
       </c>
       <c r="G9" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="J9" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -6264,150 +6241,177 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>156</v>
-      </c>
       <c r="E1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2">
+        <v>147</v>
+      </c>
+      <c r="F1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2">
         <v>123</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2345</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3">
         <v>123</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2345</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4">
         <v>123</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2345</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="16">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5">
         <v>123</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>2345</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="16">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6">
         <v>123</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>2345</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7">
         <v>123</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>2345</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8">
         <v>123</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>2345</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16">
+        <v>3000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9">
         <v>123</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>2345</v>
       </c>
-      <c r="E9" t="s">
-        <v>182</v>
+      <c r="F9" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -6417,11 +6421,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6429,925 +6433,1018 @@
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" t="s">
-        <v>158</v>
+        <v>76</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>171</v>
       </c>
       <c r="G1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>173</v>
+        <v>148</v>
+      </c>
+      <c r="I1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="K1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="L1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="M1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="16">
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="I2" s="17">
+      <c r="J2" s="17">
         <v>0.25</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="16">
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3">
+        <v>78</v>
+      </c>
+      <c r="H3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
-      <c r="I3" s="17">
+      <c r="J3" s="17">
         <v>0.95</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="16">
+        <v>3</v>
       </c>
       <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" t="s">
         <v>48</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="I4" s="17">
+      <c r="J4" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" t="s">
-        <v>82</v>
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="16">
+        <v>4</v>
       </c>
       <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" t="s">
         <v>48</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0</v>
       </c>
-      <c r="I5" s="17">
+      <c r="J5" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="16">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="I6" s="17">
+      <c r="J6" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F7" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7">
+        <v>79</v>
+      </c>
+      <c r="H7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7">
         <v>0</v>
       </c>
-      <c r="I7" s="17">
+      <c r="J7" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F8" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="16">
+        <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8">
+        <v>79</v>
+      </c>
+      <c r="H8" t="s">
+        <v>99</v>
+      </c>
+      <c r="I8">
         <v>0</v>
       </c>
-      <c r="I8" s="17">
+      <c r="J8" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="16">
+        <v>3</v>
       </c>
       <c r="G9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" t="s">
         <v>48</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="I9" s="17">
+      <c r="J9" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F10" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="16">
+        <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>127</v>
-      </c>
-      <c r="H10">
+        <v>79</v>
+      </c>
+      <c r="H10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10">
         <v>0</v>
       </c>
-      <c r="I10" s="17">
+      <c r="J10" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F11" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="16">
+        <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11">
+        <v>78</v>
+      </c>
+      <c r="H11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11">
         <v>0</v>
       </c>
-      <c r="I11" s="17">
+      <c r="J11" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F12" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H12">
+        <v>78</v>
+      </c>
+      <c r="H12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12">
         <v>0</v>
       </c>
-      <c r="I12" s="17">
+      <c r="J12" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F13" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="16">
+        <v>2</v>
       </c>
       <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" t="s">
         <v>48</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0</v>
       </c>
-      <c r="I13" s="17">
+      <c r="J13" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F14" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="16">
+        <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H14">
+        <v>78</v>
+      </c>
+      <c r="H14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I14">
         <v>0</v>
       </c>
-      <c r="I14" s="17">
+      <c r="J14" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="16">
+        <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15">
+        <v>77</v>
+      </c>
+      <c r="H15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15">
         <v>0</v>
       </c>
-      <c r="I15" s="17">
+      <c r="J15" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="16">
+        <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>101</v>
-      </c>
-      <c r="H16">
+        <v>77</v>
+      </c>
+      <c r="H16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16">
         <v>0</v>
       </c>
-      <c r="I16" s="17">
+      <c r="J16" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1</v>
       </c>
       <c r="G17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" t="s">
         <v>48</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0</v>
       </c>
-      <c r="I17" s="17">
+      <c r="J17" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F18" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="16">
+        <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>127</v>
-      </c>
-      <c r="H18">
+        <v>77</v>
+      </c>
+      <c r="H18" t="s">
+        <v>125</v>
+      </c>
+      <c r="I18">
         <v>0</v>
       </c>
-      <c r="I18" s="17">
+      <c r="J18" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="16">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" t="s">
         <v>82</v>
       </c>
-      <c r="G19" t="s">
-        <v>84</v>
-      </c>
-      <c r="H19">
+      <c r="I19">
         <v>0</v>
       </c>
-      <c r="I19" s="17">
+      <c r="J19" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F20" t="s">
-        <v>82</v>
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="16">
+        <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>101</v>
-      </c>
-      <c r="H20">
+        <v>80</v>
+      </c>
+      <c r="H20" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20">
         <v>0</v>
       </c>
-      <c r="I20" s="17">
+      <c r="J20" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F21" t="s">
-        <v>82</v>
+        <v>67</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="16">
+        <v>5</v>
       </c>
       <c r="G21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" t="s">
         <v>48</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>0</v>
       </c>
-      <c r="I21" s="17">
+      <c r="J21" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F22" t="s">
-        <v>82</v>
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="16">
+        <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H22">
+        <v>80</v>
+      </c>
+      <c r="H22" t="s">
+        <v>125</v>
+      </c>
+      <c r="I22">
         <v>0</v>
       </c>
-      <c r="I22" s="17">
+      <c r="J22" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F23" t="s">
-        <v>130</v>
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="16">
+        <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>84</v>
-      </c>
-      <c r="H23">
+        <v>128</v>
+      </c>
+      <c r="H23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23">
         <v>0</v>
       </c>
-      <c r="I23" s="17">
+      <c r="J23" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" t="s">
-        <v>130</v>
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="16">
+        <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24">
+        <v>128</v>
+      </c>
+      <c r="H24" t="s">
+        <v>99</v>
+      </c>
+      <c r="I24">
         <v>0</v>
       </c>
-      <c r="I24" s="17">
+      <c r="J24" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" t="s">
-        <v>130</v>
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="16">
+        <v>4</v>
       </c>
       <c r="G25" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" t="s">
         <v>48</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0</v>
       </c>
-      <c r="I25" s="17">
+      <c r="J25" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F26" t="s">
-        <v>130</v>
+        <v>67</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="16">
+        <v>5</v>
       </c>
       <c r="G26" t="s">
-        <v>127</v>
-      </c>
-      <c r="H26">
+        <v>128</v>
+      </c>
+      <c r="H26" t="s">
+        <v>125</v>
+      </c>
+      <c r="I26">
         <v>0</v>
       </c>
-      <c r="I26" s="17">
+      <c r="J26" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="F27" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="16">
+        <v>2000</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27">
+        <v>79</v>
+      </c>
+      <c r="H27" t="s">
+        <v>82</v>
+      </c>
+      <c r="I27">
         <v>0</v>
       </c>
-      <c r="I27" s="17">
+      <c r="J27" s="17">
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1000</v>
       </c>
       <c r="B28" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="I28" s="17">
+        <v>67</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="16">
+        <v>6</v>
+      </c>
+      <c r="J28" s="17">
         <v>1</v>
       </c>
-      <c r="J28" s="18">
+      <c r="K28" s="18">
         <v>40513</v>
       </c>
-      <c r="L28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2000</v>
       </c>
       <c r="B29" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="F29" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="16">
+        <v>2000</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
-      </c>
-      <c r="H29">
+        <v>79</v>
+      </c>
+      <c r="H29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I29">
         <v>0</v>
       </c>
-      <c r="I29" s="17">
+      <c r="J29" s="17">
         <v>0.25</v>
       </c>
-      <c r="L29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2001</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="F30" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="16">
+        <v>2000</v>
       </c>
       <c r="G30" t="s">
-        <v>84</v>
-      </c>
-      <c r="H30">
+        <v>77</v>
+      </c>
+      <c r="H30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I30">
         <v>0</v>
       </c>
-      <c r="I30" s="17">
+      <c r="J30" s="17">
         <v>0.25</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3000</v>
       </c>
       <c r="B31" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="I31" s="17">
+        <v>67</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="16">
+        <v>6</v>
+      </c>
+      <c r="J31" s="17">
         <v>1</v>
       </c>
-      <c r="J31" s="18">
+      <c r="K31" s="18">
         <v>40513</v>
       </c>
-      <c r="L31" t="s">
-        <v>179</v>
+      <c r="M31" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -7358,9 +7455,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7370,136 +7470,118 @@
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
         <v>132</v>
       </c>
-      <c r="B1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" t="s">
-        <v>57</v>
-      </c>
       <c r="I1" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="J1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="K1" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" t="s">
-        <v>155</v>
-      </c>
-      <c r="M1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B2" s="18">
         <v>42276</v>
       </c>
       <c r="C2">
-        <v>201501</v>
-      </c>
-      <c r="D2" s="16">
-        <v>2000</v>
+        <v>201504</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I2">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J2">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K2">
-        <v>221.123456</v>
-      </c>
-      <c r="L2">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M2">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B3" s="18">
         <v>42276</v>
       </c>
       <c r="C3">
-        <v>201501</v>
-      </c>
-      <c r="D3" s="16">
-        <v>2000</v>
+        <v>201504</v>
+      </c>
+      <c r="D3">
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <v>100</v>
       </c>
       <c r="H3">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I3">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J3">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K3">
-        <v>221.123456</v>
-      </c>
-      <c r="L3">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M3">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="18">
         <v>42276</v>
@@ -7511,36 +7593,30 @@
         <v>2000</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I4">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J4">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K4">
-        <v>221.123456</v>
-      </c>
-      <c r="L4">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M4">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="18">
         <v>42276</v>
@@ -7549,10 +7625,10 @@
         <v>201501</v>
       </c>
       <c r="D5" s="16">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -7561,27 +7637,21 @@
         <v>100</v>
       </c>
       <c r="H5">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I5">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J5">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K5">
-        <v>221.123456</v>
-      </c>
-      <c r="L5">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M5">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="18">
         <v>42276</v>
@@ -7590,39 +7660,33 @@
         <v>201501</v>
       </c>
       <c r="D6" s="16">
-        <v>30</v>
+        <v>2000</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H6">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I6">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J6">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K6">
-        <v>221.123456</v>
-      </c>
-      <c r="L6">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M6">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="18">
         <v>42276</v>
@@ -7631,10 +7695,10 @@
         <v>201501</v>
       </c>
       <c r="D7" s="16">
-        <v>1</v>
+        <v>2001</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -7643,121 +7707,103 @@
         <v>100</v>
       </c>
       <c r="H7">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I7">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J7">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K7">
-        <v>221.123456</v>
-      </c>
-      <c r="L7">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M7">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="18">
         <v>42276</v>
       </c>
       <c r="C8">
-        <v>201502</v>
+        <v>201501</v>
       </c>
       <c r="D8" s="16">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8">
         <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
       </c>
       <c r="G8">
         <v>100</v>
       </c>
       <c r="H8">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I8">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J8">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K8">
-        <v>221.123456</v>
-      </c>
-      <c r="L8">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M8">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="18">
         <v>42276</v>
       </c>
       <c r="C9">
-        <v>201503</v>
+        <v>201501</v>
       </c>
       <c r="D9" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>100</v>
       </c>
       <c r="H9">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I9">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J9">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K9">
-        <v>221.123456</v>
-      </c>
-      <c r="L9">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M9">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="18">
         <v>42276</v>
       </c>
       <c r="C10">
-        <v>201504</v>
+        <v>201502</v>
       </c>
       <c r="D10" s="16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -7766,68 +7812,56 @@
         <v>100</v>
       </c>
       <c r="H10">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I10">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J10">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K10">
-        <v>221.123456</v>
-      </c>
-      <c r="L10">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M10">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="18">
         <v>42276</v>
       </c>
       <c r="C11">
-        <v>201504</v>
+        <v>201503</v>
       </c>
       <c r="D11" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11">
         <v>100</v>
       </c>
       <c r="H11">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I11">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J11">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K11">
-        <v>221.123456</v>
-      </c>
-      <c r="L11">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M11">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="18">
         <v>42276</v>
@@ -7836,39 +7870,33 @@
         <v>201504</v>
       </c>
       <c r="D12" s="16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G12">
         <v>100</v>
       </c>
       <c r="H12">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I12">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J12">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K12">
-        <v>221.123456</v>
-      </c>
-      <c r="L12">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M12">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="18">
         <v>42276</v>
@@ -7877,39 +7905,33 @@
         <v>201504</v>
       </c>
       <c r="D13" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F13">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <v>100</v>
       </c>
       <c r="H13">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I13">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J13">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K13">
-        <v>221.123456</v>
-      </c>
-      <c r="L13">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M13">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="18">
         <v>42276</v>
@@ -7918,39 +7940,33 @@
         <v>201504</v>
       </c>
       <c r="D14" s="16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G14">
         <v>100</v>
       </c>
       <c r="H14">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I14">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J14">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K14">
-        <v>221.123456</v>
-      </c>
-      <c r="L14">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M14">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="18">
         <v>42276</v>
@@ -7959,51 +7975,45 @@
         <v>201504</v>
       </c>
       <c r="D15" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G15">
         <v>100</v>
       </c>
       <c r="H15">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I15">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J15">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K15">
-        <v>221.123456</v>
-      </c>
-      <c r="L15">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M15">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="18">
         <v>42276</v>
       </c>
       <c r="C16">
-        <v>201503</v>
+        <v>201504</v>
       </c>
       <c r="D16" s="16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -8012,68 +8022,56 @@
         <v>100</v>
       </c>
       <c r="H16">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I16">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J16">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K16">
-        <v>221.123456</v>
-      </c>
-      <c r="L16">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M16">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="18">
         <v>42276</v>
       </c>
       <c r="C17">
-        <v>201503</v>
+        <v>201504</v>
       </c>
       <c r="D17" s="16">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H17">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I17">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J17">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K17">
-        <v>221.123456</v>
-      </c>
-      <c r="L17">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M17">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="18">
         <v>42276</v>
@@ -8082,39 +8080,33 @@
         <v>201503</v>
       </c>
       <c r="D18" s="16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>100</v>
       </c>
       <c r="H18">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I18">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J18">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K18">
-        <v>221.123456</v>
-      </c>
-      <c r="L18">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M18">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="18">
         <v>42276</v>
@@ -8123,39 +8115,33 @@
         <v>201503</v>
       </c>
       <c r="D19" s="16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F19">
         <v>3</v>
       </c>
       <c r="G19">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H19">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I19">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J19">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K19">
-        <v>221.123456</v>
-      </c>
-      <c r="L19">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M19">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="18">
         <v>42276</v>
@@ -8164,121 +8150,103 @@
         <v>201503</v>
       </c>
       <c r="D20" s="16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G20">
         <v>100</v>
       </c>
       <c r="H20">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I20">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J20">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K20">
-        <v>221.123456</v>
-      </c>
-      <c r="L20">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M20">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="18">
         <v>42276</v>
       </c>
       <c r="C21">
-        <v>201504</v>
+        <v>201503</v>
       </c>
       <c r="D21" s="16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G21">
         <v>100</v>
       </c>
       <c r="H21">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I21">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J21">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K21">
-        <v>221.123456</v>
-      </c>
-      <c r="L21">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M21">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="18">
         <v>42276</v>
       </c>
       <c r="C22">
-        <v>201504</v>
+        <v>201503</v>
       </c>
       <c r="D22" s="16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G22">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H22">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I22">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J22">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K22">
-        <v>221.123456</v>
-      </c>
-      <c r="L22">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M22">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="18">
         <v>42276</v>
@@ -8287,39 +8255,33 @@
         <v>201504</v>
       </c>
       <c r="D23" s="16">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H23">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I23">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J23">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K23">
-        <v>221.123456</v>
-      </c>
-      <c r="L23">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M23">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="18">
         <v>42276</v>
@@ -8328,10 +8290,10 @@
         <v>201504</v>
       </c>
       <c r="D24" s="16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -8340,27 +8302,21 @@
         <v>200</v>
       </c>
       <c r="H24">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I24">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J24">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K24">
-        <v>221.123456</v>
-      </c>
-      <c r="L24">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M24">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="18">
         <v>42276</v>
@@ -8369,39 +8325,33 @@
         <v>201504</v>
       </c>
       <c r="D25" s="16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>200</v>
       </c>
       <c r="H25">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I25">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J25">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K25">
-        <v>221.123456</v>
-      </c>
-      <c r="L25">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M25">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="18">
         <v>42276</v>
@@ -8410,39 +8360,33 @@
         <v>201504</v>
       </c>
       <c r="D26" s="16">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G26">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H26">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I26">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J26">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K26">
-        <v>221.123456</v>
-      </c>
-      <c r="L26">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M26">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="18">
         <v>42276</v>
@@ -8450,40 +8394,34 @@
       <c r="C27">
         <v>201504</v>
       </c>
-      <c r="D27">
-        <v>10</v>
+      <c r="D27" s="16">
+        <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F27">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G27">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H27">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I27">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J27">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K27">
-        <v>221.123456</v>
-      </c>
-      <c r="L27">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M27">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="18">
         <v>42276</v>
@@ -8491,40 +8429,34 @@
       <c r="C28">
         <v>201504</v>
       </c>
-      <c r="D28">
-        <v>11</v>
+      <c r="D28" s="16">
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F28">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G28">
         <v>100</v>
       </c>
       <c r="H28">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I28">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J28">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K28">
-        <v>221.123456</v>
-      </c>
-      <c r="L28">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M28">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="18">
         <v>42276</v>
@@ -8533,39 +8465,33 @@
         <v>201504</v>
       </c>
       <c r="D29">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F29">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G29">
         <v>100</v>
       </c>
       <c r="H29">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I29">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J29">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K29">
-        <v>221.123456</v>
-      </c>
-      <c r="L29">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M29">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="18">
         <v>42276</v>
@@ -8574,39 +8500,33 @@
         <v>201504</v>
       </c>
       <c r="D30">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F30">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G30">
         <v>100</v>
       </c>
       <c r="H30">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I30">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J30">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K30">
-        <v>221.123456</v>
-      </c>
-      <c r="L30">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M30">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" s="18">
         <v>42276</v>
@@ -8615,39 +8535,33 @@
         <v>201504</v>
       </c>
       <c r="D31">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G31">
         <v>100</v>
       </c>
       <c r="H31">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I31">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J31">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K31">
-        <v>221.123456</v>
-      </c>
-      <c r="L31">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M31">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" s="18">
         <v>42276</v>
@@ -8656,39 +8570,33 @@
         <v>201504</v>
       </c>
       <c r="D32">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G32">
         <v>100</v>
       </c>
       <c r="H32">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I32">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J32">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K32">
-        <v>221.123456</v>
-      </c>
-      <c r="L32">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M32">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="18">
         <v>42276</v>
@@ -8697,39 +8605,33 @@
         <v>201504</v>
       </c>
       <c r="D33">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <v>100</v>
       </c>
       <c r="H33">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I33">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J33">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K33">
-        <v>221.123456</v>
-      </c>
-      <c r="L33">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M33">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="18">
         <v>42276</v>
@@ -8738,39 +8640,33 @@
         <v>201504</v>
       </c>
       <c r="D34">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <v>100</v>
       </c>
       <c r="H34">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I34">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J34">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K34">
-        <v>221.123456</v>
-      </c>
-      <c r="L34">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M34">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="18">
         <v>42276</v>
@@ -8779,39 +8675,33 @@
         <v>201504</v>
       </c>
       <c r="D35">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G35">
         <v>100</v>
       </c>
       <c r="H35">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I35">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J35">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K35">
-        <v>221.123456</v>
-      </c>
-      <c r="L35">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M35">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="18">
         <v>42276</v>
@@ -8820,37 +8710,31 @@
         <v>201504</v>
       </c>
       <c r="D36">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F36">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G36">
         <v>100</v>
       </c>
       <c r="H36">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I36">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J36">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K36">
-        <v>221.123456</v>
-      </c>
-      <c r="L36">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M36">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -8864,7 +8748,7 @@
         <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F37">
         <v>2</v>
@@ -8873,25 +8757,19 @@
         <v>100</v>
       </c>
       <c r="H37">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I37">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J37">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K37">
-        <v>221.123456</v>
-      </c>
-      <c r="L37">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M37">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -8905,7 +8783,7 @@
         <v>21</v>
       </c>
       <c r="E38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F38">
         <v>3</v>
@@ -8914,25 +8792,19 @@
         <v>100</v>
       </c>
       <c r="H38">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I38">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J38">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K38">
-        <v>221.123456</v>
-      </c>
-      <c r="L38">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M38">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -8946,7 +8818,7 @@
         <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F39">
         <v>4</v>
@@ -8955,25 +8827,19 @@
         <v>100</v>
       </c>
       <c r="H39">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I39">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J39">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K39">
-        <v>221.123456</v>
-      </c>
-      <c r="L39">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M39">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -8987,7 +8853,7 @@
         <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F40">
         <v>5</v>
@@ -8996,25 +8862,19 @@
         <v>100</v>
       </c>
       <c r="H40">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I40">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J40">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K40">
-        <v>221.123456</v>
-      </c>
-      <c r="L40">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M40">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -9028,7 +8888,7 @@
         <v>24</v>
       </c>
       <c r="E41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F41">
         <v>6</v>
@@ -9037,25 +8897,19 @@
         <v>100</v>
       </c>
       <c r="H41">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I41">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J41">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K41">
-        <v>221.123456</v>
-      </c>
-      <c r="L41">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M41">
         <v>0.123455</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -9069,7 +8923,7 @@
         <v>25</v>
       </c>
       <c r="E42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F42">
         <v>2</v>
@@ -9078,21 +8932,15 @@
         <v>100</v>
       </c>
       <c r="H42">
-        <v>100</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I42">
-        <v>200</v>
+        <v>221.123456</v>
       </c>
       <c r="J42">
-        <v>2.2000000000000002</v>
+        <v>2.1234549999999999</v>
       </c>
       <c r="K42">
-        <v>221.123456</v>
-      </c>
-      <c r="L42">
-        <v>2.1234549999999999</v>
-      </c>
-      <c r="M42">
         <v>0.123455</v>
       </c>
     </row>
@@ -9116,13 +8964,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -9130,7 +8978,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>0.25</v>
@@ -9156,10 +9004,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -9189,28 +9037,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
       <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
         <v>61</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- start on GORR - add DataDic Tab
</commit_message>
<xml_diff>
--- a/excel-app/database.xlsx
+++ b/excel-app/database.xlsx
@@ -9,26 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
     <sheet name="ReferenceData" sheetId="3" r:id="rId2"/>
-    <sheet name="RoyaltyMaster" sheetId="2" r:id="rId3"/>
-    <sheet name="Lease" sheetId="4" r:id="rId4"/>
-    <sheet name="Well" sheetId="9" r:id="rId5"/>
-    <sheet name="Monthly" sheetId="5" r:id="rId6"/>
-    <sheet name="ProducingEntity" sheetId="11" r:id="rId7"/>
-    <sheet name="ExternalValues" sheetId="6" r:id="rId8"/>
-    <sheet name="ProductClauses" sheetId="7" r:id="rId9"/>
-    <sheet name="ECONData" sheetId="10" r:id="rId10"/>
+    <sheet name="DataDict" sheetId="12" r:id="rId3"/>
+    <sheet name="RoyaltyMaster" sheetId="2" r:id="rId4"/>
+    <sheet name="Lease" sheetId="4" r:id="rId5"/>
+    <sheet name="Well" sheetId="9" r:id="rId6"/>
+    <sheet name="Monthly" sheetId="5" r:id="rId7"/>
+    <sheet name="ProducingEntity" sheetId="11" r:id="rId8"/>
+    <sheet name="ExternalValues" sheetId="6" r:id="rId9"/>
+    <sheet name="ProductClauses" sheetId="7" r:id="rId10"/>
+    <sheet name="ECONData" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="184">
   <si>
     <t>Lease Type</t>
   </si>
@@ -544,13 +545,52 @@
   </si>
   <si>
     <t>LeaseID</t>
+  </si>
+  <si>
+    <t>Lease</t>
+  </si>
+  <si>
+    <t>The Lease ID is a numeric number. Please see Myrna for the next available number. Bla bla bla</t>
+  </si>
+  <si>
+    <t>Lazutin, Konstantin</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>Wieler, Kevin</t>
+  </si>
+  <si>
+    <t>Gorr</t>
+  </si>
+  <si>
+    <t>mprod,250,2,300,3,400,4,500,5,0,6</t>
+  </si>
+  <si>
+    <t>dprod,250,2,300,3,400,4,500,5,0,6</t>
+  </si>
+  <si>
+    <t>fixed,0,2</t>
+  </si>
+  <si>
+    <t>RoyaltyMaster</t>
+  </si>
+  <si>
+    <t>GORR can be based on monthly production mprod, daily production (monthly production / hours producing / 24) dprod, or a fixed percent fixed. Leave the last volume as zero (meaning all the rest).</t>
+  </si>
+  <si>
+    <t>SKProvCrownVar, GORR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,16 +618,36 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -681,11 +741,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -732,8 +811,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -803,6 +917,226 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="checkPrintingReportForm:checkListTable:0:payMethodIcon0" descr="https://qbo-ca.onlinepayroll.intuit.com/resources/images/harmony/payMethod_check.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8048625" y="5143500"/>
+          <a:ext cx="152400" cy="104775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="checkPrintingReportForm:checkListTable:1:payMethodIcon0" descr="https://qbo-ca.onlinepayroll.intuit.com/resources/images/harmony/payMethod_check.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10144125" y="5334000"/>
+          <a:ext cx="152400" cy="104775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="checkPrintingReportForm:checkListTable:2:payMethodIcon0" descr="https://qbo-ca.onlinepayroll.intuit.com/resources/images/harmony/payMethod_check.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10144125" y="5524500"/>
+          <a:ext cx="152400" cy="104775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="checkPrintingReportForm:checkListTable:3:payMethodIcon0" descr="https://qbo-ca.onlinepayroll.intuit.com/resources/images/harmony/payMethod_check.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10144125" y="5715000"/>
+          <a:ext cx="152400" cy="104775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1095,10 +1429,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,22 +1643,22 @@
       <c r="G15" s="9"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>43</v>
       </c>
@@ -1331,7 +1666,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>44</v>
       </c>
@@ -1339,24 +1674,163 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>48</v>
       </c>
     </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="21">
+        <v>42307</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E28" s="23">
+        <v>3559.12</v>
+      </c>
+      <c r="F28" s="24">
+        <v>2909.71</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H28" s="20"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="22"/>
+      <c r="C29" s="21">
+        <v>42307</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="E29" s="23">
+        <v>12092.5</v>
+      </c>
+      <c r="F29" s="24">
+        <v>11281.02</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H29" s="25"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="22"/>
+      <c r="C30" s="21">
+        <v>42282</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E30" s="23">
+        <v>4000</v>
+      </c>
+      <c r="F30" s="24">
+        <v>2795.11</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H30" s="25"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="26"/>
+      <c r="C31" s="27">
+        <v>42282</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" s="28">
+        <v>164</v>
+      </c>
+      <c r="F31" s="29">
+        <v>114.6</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="H31" s="30"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f>SUM(E27:E32)</f>
+        <v>19815.62</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F28" r:id="rId1" display="https://qbo-ca.onlinepayroll.intuit.com/reports/checkRegister.jsf?directAccess=true"/>
+    <hyperlink ref="F29" r:id="rId2" display="https://qbo-ca.onlinepayroll.intuit.com/reports/checkRegister.jsf?directAccess=true"/>
+    <hyperlink ref="F30" r:id="rId3" display="https://qbo-ca.onlinepayroll.intuit.com/reports/checkRegister.jsf?directAccess=true"/>
+    <hyperlink ref="F31" r:id="rId4" display="https://qbo-ca.onlinepayroll.intuit.com/reports/checkRegister.jsf?directAccess=true"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE48"/>
   <sheetViews>
@@ -5998,10 +6472,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6009,13 +6524,14 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="10" max="10" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>52</v>
       </c>
@@ -6044,10 +6560,13 @@
         <v>134</v>
       </c>
       <c r="J1" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6058,7 +6577,7 @@
         <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="E2">
         <v>1.2</v>
@@ -6075,8 +6594,11 @@
       <c r="I2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6101,8 +6623,11 @@
       <c r="H3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -6124,8 +6649,11 @@
       <c r="I4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -6151,7 +6679,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -6171,7 +6699,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -6191,7 +6719,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -6211,7 +6739,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -6230,7 +6758,7 @@
       <c r="G9" t="s">
         <v>154</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>169</v>
       </c>
     </row>
@@ -6239,7 +6767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -6419,12 +6947,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -7453,11 +7981,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -8949,7 +9477,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -8989,7 +9517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -9013,55 +9541,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- write royalty calc record to worksheet
</commit_message>
<xml_diff>
--- a/excel-app/database.xlsx
+++ b/excel-app/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,20 @@
     <sheet name="RoyaltyMaster" sheetId="2" r:id="rId4"/>
     <sheet name="Lease" sheetId="4" r:id="rId5"/>
     <sheet name="Well" sheetId="9" r:id="rId6"/>
-    <sheet name="Monthly" sheetId="5" r:id="rId7"/>
-    <sheet name="ProducingEntity" sheetId="11" r:id="rId8"/>
-    <sheet name="ExternalValues" sheetId="6" r:id="rId9"/>
-    <sheet name="ProductClauses" sheetId="7" r:id="rId10"/>
-    <sheet name="ECONData" sheetId="10" r:id="rId11"/>
+    <sheet name="MonthlyLots" sheetId="5" r:id="rId7"/>
+    <sheet name="Monthly" sheetId="13" r:id="rId8"/>
+    <sheet name="Calc" sheetId="14" r:id="rId9"/>
+    <sheet name="ProducingEntity" sheetId="11" r:id="rId10"/>
+    <sheet name="ExternalValues" sheetId="6" r:id="rId11"/>
+    <sheet name="ProductClauses" sheetId="7" r:id="rId12"/>
+    <sheet name="ECONData" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="209">
   <si>
     <t>Lease Type</t>
   </si>
@@ -584,6 +586,78 @@
   </si>
   <si>
     <t>IOGR1995, GORR</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>RoyaltyPrice</t>
+  </si>
+  <si>
+    <t>RoyaltyVolume</t>
+  </si>
+  <si>
+    <t>ProvCrownRoyaltyRate</t>
+  </si>
+  <si>
+    <t>ProvCrownUsedRoyaltyRate</t>
+  </si>
+  <si>
+    <t>IOGR1995RoyaltyRate</t>
+  </si>
+  <si>
+    <t>GorrRoyaltyRate</t>
+  </si>
+  <si>
+    <t>ProvCrownRoyaltyVolume</t>
+  </si>
+  <si>
+    <t>GorrRoyaltyVolume</t>
+  </si>
+  <si>
+    <t>IOGR1995RoyaltyVolume</t>
+  </si>
+  <si>
+    <t>ProvCrownRoyaltyValue</t>
+  </si>
+  <si>
+    <t>IOGR1995RoyaltyValue</t>
+  </si>
+  <si>
+    <t>GorrRoyaltyValue</t>
+  </si>
+  <si>
+    <t>RoyaltyValuePreDeductions</t>
+  </si>
+  <si>
+    <t>RoyaltyTransportation</t>
+  </si>
+  <si>
+    <t>RoyaltyProcessing</t>
+  </si>
+  <si>
+    <t>RoyaltyDeductions</t>
+  </si>
+  <si>
+    <t>RoyaltyValue</t>
+  </si>
+  <si>
+    <t>CommencementPeriod</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>GorrMessage</t>
   </si>
 </sst>
 </file>
@@ -1788,6 +1862,72 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1837,7 +1977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE48"/>
   <sheetViews>
@@ -6522,8 +6662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8164,7 +8304,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9897,37 +10037,91 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D27" sqref="D27:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>70</v>
+      <c r="B2" s="18">
+        <v>42276</v>
       </c>
       <c r="C2">
-        <v>0.25</v>
+        <v>201501</v>
+      </c>
+      <c r="D2" s="16">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>740</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J2">
+        <v>221.123456</v>
+      </c>
+      <c r="K2">
+        <v>2.1234549999999999</v>
+      </c>
+      <c r="L2">
+        <v>0.123455</v>
       </c>
     </row>
   </sheetData>
@@ -9937,23 +10131,92 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>199</v>
+      </c>
+      <c r="R1" t="s">
+        <v>200</v>
+      </c>
+      <c r="S1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T1" t="s">
+        <v>202</v>
+      </c>
+      <c r="U1" t="s">
+        <v>203</v>
+      </c>
+      <c r="V1" t="s">
+        <v>204</v>
+      </c>
+      <c r="W1" t="s">
+        <v>205</v>
+      </c>
+      <c r="X1" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>207</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>